<commit_message>
compare-implan-sectoring and update package implan 1.1
</commit_message>
<xml_diff>
--- a/data/processed/category_to_sector546.xlsx
+++ b/data/processed/category_to_sector546.xlsx
@@ -7,10 +7,10 @@
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="8" state="visible" r:id="rId1"/>
-    <sheet name="oia" sheetId="34" state="visible" r:id="rId2"/>
-    <sheet name="fish" sheetId="35" state="visible" r:id="rId3"/>
-    <sheet name="hunt" sheetId="36" state="visible" r:id="rId4"/>
-    <sheet name="wildlife" sheetId="37" state="visible" r:id="rId5"/>
+    <sheet name="oia" sheetId="38" state="visible" r:id="rId2"/>
+    <sheet name="fish" sheetId="39" state="visible" r:id="rId3"/>
+    <sheet name="hunt" sheetId="40" state="visible" r:id="rId4"/>
+    <sheet name="wildlife" sheetId="41" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>